<commit_message>
mainpage improvements, error prevention
</commit_message>
<xml_diff>
--- a/2_Documentation/Time.xlsx
+++ b/2_Documentation/Time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\RcTireManager\2_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45CD50DA-8C89-4577-91C1-C6A379EF086B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05850405-0011-43AB-B4F2-DA4246EFD11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14220" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{39767669-6BA0-42DD-8828-B91135BB5742}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="19200" windowHeight="11180" xr2:uid="{39767669-6BA0-42DD-8828-B91135BB5742}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -434,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66368104-ED64-4BE9-918C-19095C93BABA}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -462,7 +462,7 @@
       </c>
       <c r="D2">
         <f>SUM(B:B)</f>
-        <v>17.350000000000001</v>
+        <v>18.350000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
@@ -539,10 +539,18 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="1">
-        <v>46042</v>
+        <v>46046</v>
       </c>
       <c r="B12">
-        <v>2.5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A13" s="1">
+        <v>46047</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cards for tires and cars
</commit_message>
<xml_diff>
--- a/2_Documentation/Time.xlsx
+++ b/2_Documentation/Time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\RcTireManager\2_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4C0589-87AC-4A4B-891F-46404F2AFC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D484F3F-90E6-4813-9B00-2172C6A5DC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="19200" windowHeight="11180" xr2:uid="{39767669-6BA0-42DD-8828-B91135BB5742}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11100" xr2:uid="{39767669-6BA0-42DD-8828-B91135BB5742}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -434,15 +434,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66368104-ED64-4BE9-918C-19095C93BABA}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -453,7 +453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45927</v>
       </c>
@@ -462,10 +462,10 @@
       </c>
       <c r="D2">
         <f>SUM(B:B)</f>
-        <v>19.350000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+        <v>20.350000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45929</v>
       </c>
@@ -473,7 +473,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45930</v>
       </c>
@@ -481,7 +481,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45901</v>
       </c>
@@ -489,7 +489,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45942</v>
       </c>
@@ -497,7 +497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45943</v>
       </c>
@@ -505,7 +505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45994</v>
       </c>
@@ -513,7 +513,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45995</v>
       </c>
@@ -521,7 +521,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>46000</v>
       </c>
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>46008</v>
       </c>
@@ -537,7 +537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>46046</v>
       </c>
@@ -545,7 +545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>46047</v>
       </c>
@@ -553,11 +553,19 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>46047</v>
       </c>
       <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>46048</v>
+      </c>
+      <c r="B15">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data context code cleanup
</commit_message>
<xml_diff>
--- a/2_Documentation/Time.xlsx
+++ b/2_Documentation/Time.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\RcTireManager\2_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0919EB03-3348-4BD0-8988-974B7E6C7A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161C97BD-DDA9-4D4A-AA5A-8C8409B31F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1073" yWindow="1073" windowWidth="19200" windowHeight="11180" xr2:uid="{39767669-6BA0-42DD-8828-B91135BB5742}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{39767669-6BA0-42DD-8828-B91135BB5742}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -443,18 +443,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66368104-ED64-4BE9-918C-19095C93BABA}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.8203125" style="4"/>
+    <col min="1" max="16384" width="10.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>45927</v>
       </c>
@@ -474,10 +474,10 @@
       </c>
       <c r="D2" s="4">
         <f>SUM(B:B)</f>
-        <v>22.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>45929</v>
       </c>
@@ -485,7 +485,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>45930</v>
       </c>
@@ -493,7 +493,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>45901</v>
       </c>
@@ -501,7 +501,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>45942</v>
       </c>
@@ -509,7 +509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>45943</v>
       </c>
@@ -517,7 +517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>45994</v>
       </c>
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>45995</v>
       </c>
@@ -533,7 +533,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>46000</v>
       </c>
@@ -541,7 +541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>46008</v>
       </c>
@@ -549,7 +549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>46046</v>
       </c>
@@ -557,7 +557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>46047</v>
       </c>
@@ -565,7 +565,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>46047</v>
       </c>
@@ -573,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>46048</v>
       </c>
@@ -581,7 +581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>46051</v>
       </c>
@@ -589,12 +589,20 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>46051</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>46055</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>